<commit_message>
Deleted unnecessary files (.DS_Store, names.xlsx, ~.xlsx, 23.xlsx, checker.py) from the project.
</commit_message>
<xml_diff>
--- a/colleagues.xlsx
+++ b/colleagues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MimounB/Desktop/VScode/openspace-organizer-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53331DB-380D-BF43-B451-4D0F15A8B506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDA6417-7948-A04F-B43F-A6AEE8B3AE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Names</t>
   </si>
@@ -92,24 +92,6 @@
   </si>
   <si>
     <t>Cisco</t>
-  </si>
-  <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quinten </t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>Tony</t>
-  </si>
-  <si>
-    <t>Julian</t>
-  </si>
-  <si>
-    <t>Dany</t>
   </si>
 </sst>
 </file>
@@ -477,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -602,36 +584,6 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>